<commit_message>
w3d1 - practice complete
</commit_message>
<xml_diff>
--- a/week_3/spreadsheets/w3_d1_practice.xlsx
+++ b/week_3/spreadsheets/w3_d1_practice.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,19 +423,46 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>clefairy</t>
+        </is>
+      </c>
+      <c r="C1" t="n">
+        <v>113</v>
+      </c>
+      <c r="D1" t="n">
+        <v>6</v>
+      </c>
+      <c r="E1" t="n">
+        <v>56</v>
+      </c>
+      <c r="F1" t="n">
         <v>75</v>
       </c>
-      <c r="B1" t="n">
-        <v>75</v>
-      </c>
-      <c r="C1" t="n">
-        <v>75</v>
-      </c>
-      <c r="D1" t="n">
-        <v>75</v>
-      </c>
-      <c r="E1" t="n">
-        <v>75</v>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>13</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>weedle</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>39</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" t="n">
+        <v>17</v>
+      </c>
+      <c r="F2" t="n">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>